<commit_message>
Sat Jan 25 02:21:20 PM EST 2025 re-run ozone ANO-RCC-MB
</commit_message>
<xml_diff>
--- a/ozone/ANO-RCC-MB/ozone_106.00/ozone_106.00_energies.xlsx
+++ b/ozone/ANO-RCC-MB/ozone_106.00/ozone_106.00_energies.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.0939261435</v>
+        <v>-0.09393797800000001</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-224.35978288</v>
+        <v>-224.35978283</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-224.45370902</v>
+        <v>-224.45372081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>